<commit_message>
fix(multiple): working for multiple rivers
Signed-off-by: guilhermedurbano <guilhermedurbano@gmail.com>
</commit_message>
<xml_diff>
--- a/data/preprocessing/departure_patterns/14_days.xlsx
+++ b/data/preprocessing/departure_patterns/14_days.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\src\tcc-GNL-amazon\data\preprocessing\departure_patterns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\tcc-GNL-amazon\data\preprocessing\departure_patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715AA836-2417-4170-8A02-E5E836F53451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF7488-90C4-445B-909D-BBC9D6606154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC129893-5089-43D2-9B4A-D458CA2F4A93}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC129893-5089-43D2-9B4A-D458CA2F4A93}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -153,11 +153,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -173,11 +184,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -487,18 +511,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9B64BD-8D7C-457D-A147-3C4B2B03EF4D}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="10"/>
+    <col min="2" max="2" width="9.109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -548,7 +572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -599,7 +623,7 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -650,7 +674,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -701,7 +725,7 @@
       </c>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -752,7 +776,7 @@
       </c>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -803,7 +827,7 @@
       </c>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -854,7 +878,7 @@
       </c>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -905,7 +929,7 @@
       </c>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -956,7 +980,7 @@
       </c>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1007,7 +1031,7 @@
       </c>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1058,7 +1082,7 @@
       </c>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1109,7 +1133,7 @@
       </c>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1160,7 +1184,7 @@
       </c>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1211,7 +1235,7 @@
       </c>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1262,7 +1286,7 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1313,7 +1337,7 @@
       </c>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1364,7 +1388,7 @@
       </c>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1415,7 +1439,7 @@
       </c>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1466,7 +1490,7 @@
       </c>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1517,7 +1541,7 @@
       </c>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1568,7 +1592,7 @@
       </c>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1619,7 +1643,7 @@
       </c>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1670,7 +1694,7 @@
       </c>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1721,7 +1745,7 @@
       </c>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1772,7 +1796,7 @@
       </c>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1823,7 +1847,7 @@
       </c>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1874,7 +1898,7 @@
       </c>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1925,7 +1949,7 @@
       </c>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1976,7 +2000,7 @@
       </c>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2027,7 +2051,7 @@
       </c>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2078,7 +2102,7 @@
       </c>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2129,7 +2153,7 @@
       </c>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2180,7 +2204,7 @@
       </c>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2231,7 +2255,7 @@
       </c>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2282,7 +2306,7 @@
       </c>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2333,7 +2357,7 @@
       </c>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2359,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="I37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="4">
         <v>0</v>
@@ -2384,7 +2408,7 @@
       </c>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2394,40 +2418,40 @@
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="14">
-        <v>0</v>
-      </c>
-      <c r="E38" s="14">
-        <v>0</v>
-      </c>
-      <c r="F38" s="14">
-        <v>0</v>
-      </c>
-      <c r="G38" s="14">
-        <v>1</v>
-      </c>
-      <c r="H38" s="14">
-        <v>0</v>
-      </c>
-      <c r="I38" s="14">
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
         <v>0</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
       </c>
-      <c r="K38" s="14">
-        <v>0</v>
-      </c>
-      <c r="L38" s="14">
-        <v>0</v>
-      </c>
-      <c r="M38" s="14">
-        <v>0</v>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>1</v>
       </c>
       <c r="N38" s="1">
-        <v>1</v>
-      </c>
-      <c r="O38" s="14">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
         <v>0</v>
       </c>
       <c r="P38" s="7">
@@ -2435,7 +2459,7 @@
       </c>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2443,42 +2467,42 @@
         <v>4</v>
       </c>
       <c r="C39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="14">
-        <v>0</v>
-      </c>
-      <c r="F39" s="14">
-        <v>0</v>
-      </c>
-      <c r="G39" s="14">
-        <v>1</v>
-      </c>
-      <c r="H39" s="14">
-        <v>0</v>
-      </c>
-      <c r="I39" s="14">
-        <v>0</v>
-      </c>
-      <c r="J39" s="14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1</v>
       </c>
       <c r="K39" s="1">
-        <v>1</v>
-      </c>
-      <c r="L39" s="14">
-        <v>0</v>
-      </c>
-      <c r="M39" s="14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1</v>
       </c>
       <c r="N39" s="1">
-        <v>1</v>
-      </c>
-      <c r="O39" s="14">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
         <v>0</v>
       </c>
       <c r="P39" s="7">
@@ -2486,58 +2510,58 @@
       </c>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="12">
         <v>4</v>
       </c>
       <c r="C40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="14">
-        <v>0</v>
-      </c>
-      <c r="F40" s="14">
-        <v>0</v>
-      </c>
-      <c r="G40" s="14">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>1</v>
-      </c>
-      <c r="I40" s="14">
-        <v>0</v>
-      </c>
-      <c r="J40" s="14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
       </c>
       <c r="K40" s="1">
-        <v>1</v>
-      </c>
-      <c r="L40" s="14">
-        <v>0</v>
-      </c>
-      <c r="M40" s="14">
-        <v>0</v>
-      </c>
-      <c r="N40" s="14">
-        <v>0</v>
-      </c>
-      <c r="O40" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1</v>
+      </c>
+      <c r="O40" s="14">
+        <v>0</v>
       </c>
       <c r="P40" s="7">
         <v>0</v>
       </c>
-      <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q40" s="14"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2545,49 +2569,50 @@
         <v>4</v>
       </c>
       <c r="C41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="14">
         <v>0</v>
       </c>
-      <c r="E41" s="1">
-        <v>1</v>
+      <c r="E41" s="14">
+        <v>0</v>
       </c>
       <c r="F41" s="14">
         <v>0</v>
       </c>
       <c r="G41" s="14">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H41" s="14">
+        <v>0</v>
       </c>
       <c r="I41" s="14">
         <v>0</v>
       </c>
-      <c r="J41" s="14">
-        <v>0</v>
+      <c r="J41" s="1">
+        <v>1</v>
       </c>
       <c r="K41" s="14">
         <v>0</v>
       </c>
-      <c r="L41" s="1">
-        <v>1</v>
+      <c r="L41" s="14">
+        <v>0</v>
       </c>
       <c r="M41" s="14">
         <v>0</v>
       </c>
-      <c r="N41" s="14">
-        <v>0</v>
-      </c>
-      <c r="O41" s="1">
-        <v>1</v>
+      <c r="N41" s="1">
+        <v>1</v>
+      </c>
+      <c r="O41" s="14">
+        <v>0</v>
       </c>
       <c r="P41" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q41" s="14"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2595,49 +2620,50 @@
         <v>4</v>
       </c>
       <c r="C42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="14">
         <v>0</v>
       </c>
-      <c r="E42" s="1">
-        <v>1</v>
+      <c r="E42" s="14">
+        <v>0</v>
       </c>
       <c r="F42" s="14">
         <v>0</v>
       </c>
-      <c r="G42" s="14">
-        <v>0</v>
+      <c r="G42" s="1">
+        <v>1</v>
       </c>
       <c r="H42" s="14">
         <v>0</v>
       </c>
-      <c r="I42" s="1">
-        <v>1</v>
+      <c r="I42" s="14">
+        <v>0</v>
       </c>
       <c r="J42" s="14">
         <v>0</v>
       </c>
       <c r="K42" s="14">
-        <v>0</v>
-      </c>
-      <c r="L42" s="1">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="L42" s="14">
+        <v>0</v>
       </c>
       <c r="M42" s="14">
         <v>0</v>
       </c>
       <c r="N42" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O42" s="14">
         <v>0</v>
       </c>
-      <c r="P42" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P42" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="14"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2647,47 +2673,753 @@
       <c r="C43" s="6">
         <v>0</v>
       </c>
-      <c r="D43" s="14">
-        <v>0</v>
-      </c>
-      <c r="E43" s="14">
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="14">
-        <v>0</v>
-      </c>
-      <c r="H43" s="14">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
         <v>0</v>
       </c>
       <c r="I43" s="1">
-        <v>1</v>
-      </c>
-      <c r="J43" s="14">
-        <v>0</v>
-      </c>
-      <c r="K43" s="14">
-        <v>0</v>
-      </c>
-      <c r="L43" s="14">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1">
         <v>0</v>
       </c>
       <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="14">
-        <v>0</v>
-      </c>
-      <c r="O43" s="14">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1">
         <v>0</v>
       </c>
       <c r="P43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="16">
+        <v>4</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0</v>
+      </c>
+      <c r="P44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="12">
+        <v>4</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0</v>
+      </c>
+      <c r="N45" s="1">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1">
+        <v>0</v>
+      </c>
+      <c r="P45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="12">
+        <v>4</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0</v>
+      </c>
+      <c r="N46" s="1">
+        <v>0</v>
+      </c>
+      <c r="O46" s="1">
+        <v>1</v>
+      </c>
+      <c r="P46" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="12">
+        <v>4</v>
+      </c>
+      <c r="C47" s="6">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="14">
+        <v>0</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0</v>
+      </c>
+      <c r="G47" s="14">
+        <v>0</v>
+      </c>
+      <c r="H47" s="14">
+        <v>1</v>
+      </c>
+      <c r="I47" s="14">
+        <v>0</v>
+      </c>
+      <c r="J47" s="14">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0</v>
+      </c>
+      <c r="M47" s="14">
+        <v>0</v>
+      </c>
+      <c r="N47" s="14">
+        <v>0</v>
+      </c>
+      <c r="O47" s="1">
+        <v>1</v>
+      </c>
+      <c r="P47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" s="12">
+        <v>4</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="14">
+        <v>0</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0</v>
+      </c>
+      <c r="G48" s="14">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>1</v>
+      </c>
+      <c r="I48" s="14">
+        <v>0</v>
+      </c>
+      <c r="J48" s="14">
+        <v>0</v>
+      </c>
+      <c r="K48" s="14">
+        <v>0</v>
+      </c>
+      <c r="L48" s="14">
+        <v>1</v>
+      </c>
+      <c r="M48" s="14">
+        <v>0</v>
+      </c>
+      <c r="N48" s="14">
+        <v>0</v>
+      </c>
+      <c r="O48" s="14">
+        <v>1</v>
+      </c>
+      <c r="P48" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" s="12">
+        <v>4</v>
+      </c>
+      <c r="C49" s="6">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0</v>
+      </c>
+      <c r="O49" s="1">
+        <v>1</v>
+      </c>
+      <c r="P49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" s="12">
+        <v>4</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1">
+        <v>1</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
+      <c r="N50" s="1">
+        <v>0</v>
+      </c>
+      <c r="O50" s="1">
+        <v>1</v>
+      </c>
+      <c r="P50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" s="12">
+        <v>4</v>
+      </c>
+      <c r="C51" s="6">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0</v>
+      </c>
+      <c r="L51" s="1">
+        <v>1</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0</v>
+      </c>
+      <c r="O51" s="1">
+        <v>1</v>
+      </c>
+      <c r="P51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="12">
+        <v>4</v>
+      </c>
+      <c r="C52" s="6">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0</v>
+      </c>
+      <c r="O52" s="1">
+        <v>0</v>
+      </c>
+      <c r="P52" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" s="12">
+        <v>4</v>
+      </c>
+      <c r="C53" s="6">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="14">
+        <v>0</v>
+      </c>
+      <c r="G53" s="14">
+        <v>0</v>
+      </c>
+      <c r="H53" s="14">
+        <v>0</v>
+      </c>
+      <c r="I53" s="14">
+        <v>1</v>
+      </c>
+      <c r="J53" s="14">
+        <v>0</v>
+      </c>
+      <c r="K53" s="14">
+        <v>0</v>
+      </c>
+      <c r="L53" s="1">
+        <v>1</v>
+      </c>
+      <c r="M53" s="14">
+        <v>0</v>
+      </c>
+      <c r="N53" s="14">
+        <v>0</v>
+      </c>
+      <c r="O53" s="14">
+        <v>0</v>
+      </c>
+      <c r="P53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" s="12">
+        <v>4</v>
+      </c>
+      <c r="C54" s="6">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="14">
+        <v>0</v>
+      </c>
+      <c r="G54" s="14">
+        <v>0</v>
+      </c>
+      <c r="H54" s="14">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <v>1</v>
+      </c>
+      <c r="J54" s="14">
+        <v>0</v>
+      </c>
+      <c r="K54" s="14">
+        <v>0</v>
+      </c>
+      <c r="L54" s="14">
+        <v>0</v>
+      </c>
+      <c r="M54" s="14">
+        <v>1</v>
+      </c>
+      <c r="N54" s="14">
+        <v>0</v>
+      </c>
+      <c r="O54" s="14">
+        <v>0</v>
+      </c>
+      <c r="P54" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" s="12">
+        <v>4</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1">
+        <v>0</v>
+      </c>
+      <c r="L55" s="1">
+        <v>1</v>
+      </c>
+      <c r="M55" s="1">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
+      </c>
+      <c r="O55" s="1">
+        <v>0</v>
+      </c>
+      <c r="P55" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" s="12">
+        <v>4</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <v>0</v>
+      </c>
+      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+      <c r="M56" s="1">
+        <v>1</v>
+      </c>
+      <c r="N56" s="1">
+        <v>0</v>
+      </c>
+      <c r="O56" s="1">
+        <v>0</v>
+      </c>
+      <c r="P56" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" s="13">
+        <v>4</v>
+      </c>
+      <c r="C57" s="8">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2">
+        <v>1</v>
+      </c>
+      <c r="K57" s="2">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2">
+        <v>1</v>
+      </c>
+      <c r="N57" s="2">
+        <v>0</v>
+      </c>
+      <c r="O57" s="2">
+        <v>0</v>
+      </c>
+      <c r="P57" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C79:M83 C58:E78 C2:P57">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>